<commit_message>
minor changes - Marc brench
</commit_message>
<xml_diff>
--- a/data/Yxs_table.xlsx
+++ b/data/Yxs_table.xlsx
@@ -1005,7 +1005,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>19.2</v>
+        <v>23.16</v>
       </c>
       <c r="B21" t="n">
         <v>42</v>
@@ -1016,7 +1016,7 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
-        <v>-0.07943046883992988</v>
+        <v>-0.08391650648756285</v>
       </c>
       <c r="I21" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
LHS_samples in objective function
</commit_message>
<xml_diff>
--- a/data/Yxs_table.xlsx
+++ b/data/Yxs_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,22 +471,32 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>mu [1/h]</t>
+          <t>mu 1 [1/h]</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Yxs 1 [gx/gs]</t>
+          <t>mu 2 [1/h]</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Yxs 2 [gx/gs]</t>
+          <t>Yxs 1.1 [gx/gs]</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Yxs 3 [gx/gs]</t>
+          <t>Yxs 1.2 [gx/gs]</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Yxs 2.1 [gx/gs]</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Yxs 2.2 [gx/gs]</t>
         </is>
       </c>
     </row>
@@ -516,6 +526,8 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -543,12 +555,18 @@
         <v>0.3346417012349824</v>
       </c>
       <c r="I3" t="n">
-        <v>-14.0151515227274</v>
+        <v>0.3346417012349824</v>
       </c>
       <c r="J3" t="n">
         <v>-14.0151515227274</v>
       </c>
       <c r="K3" t="n">
+        <v>14.0151515227274</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-14.0151515227274</v>
+      </c>
+      <c r="M3" t="n">
         <v>14.0151515227274</v>
       </c>
     </row>
@@ -578,12 +596,18 @@
         <v>0.3801731398173669</v>
       </c>
       <c r="I4" t="n">
+        <v>0.8127218063500202</v>
+      </c>
+      <c r="J4" t="n">
         <v>-38.54545454545568</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
+        <v>38.54545454545568</v>
+      </c>
+      <c r="L4" t="n">
         <v>10.51515149999989</v>
       </c>
-      <c r="K4" t="n">
+      <c r="M4" t="n">
         <v>10.51515149999989</v>
       </c>
     </row>
@@ -613,12 +637,18 @@
         <v>0.3953667590144278</v>
       </c>
       <c r="I5" t="n">
+        <v>0.4243727592997257</v>
+      </c>
+      <c r="J5" t="n">
         <v>-3.299688472897195</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
+        <v>3.299688472897195</v>
+      </c>
+      <c r="L5" t="n">
         <v>-1.788174138401557</v>
       </c>
-      <c r="K5" t="n">
+      <c r="M5" t="n">
         <v>1.788174138401557</v>
       </c>
     </row>
@@ -648,12 +678,18 @@
         <v>0.3666255505270102</v>
       </c>
       <c r="I6" t="n">
+        <v>0.2746536833672744</v>
+      </c>
+      <c r="J6" t="n">
         <v>-2.568350168686871</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
+        <v>2.568350168686871</v>
+      </c>
+      <c r="L6" t="n">
         <v>-1.708424909890113</v>
       </c>
-      <c r="K6" t="n">
+      <c r="M6" t="n">
         <v>1.708424909890113</v>
       </c>
     </row>
@@ -683,12 +719,18 @@
         <v>0.3256027443493761</v>
       </c>
       <c r="I7" t="n">
+        <v>0.1442387591429934</v>
+      </c>
+      <c r="J7" t="n">
         <v>-1.73448275862069</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
+        <v>1.73448275862069</v>
+      </c>
+      <c r="L7" t="n">
         <v>-0.633777777333333</v>
       </c>
-      <c r="K7" t="n">
+      <c r="M7" t="n">
         <v>0.633777777333333</v>
       </c>
     </row>
@@ -718,12 +760,18 @@
         <v>0.3087089219303946</v>
       </c>
       <c r="I8" t="n">
+        <v>0.2217057364726398</v>
+      </c>
+      <c r="J8" t="n">
         <v>-1.684195525010689</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
+        <v>1.684195525010689</v>
+      </c>
+      <c r="L8" t="n">
         <v>-1.538119086811352</v>
       </c>
-      <c r="K8" t="n">
+      <c r="M8" t="n">
         <v>1.538119086811352</v>
       </c>
     </row>
@@ -753,12 +801,18 @@
         <v>0.2777536623127322</v>
       </c>
       <c r="I9" t="n">
+        <v>0.07735908689312881</v>
+      </c>
+      <c r="J9" t="n">
         <v>-1.340620445658963</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
+        <v>1.340620445658963</v>
+      </c>
+      <c r="L9" t="n">
         <v>-0.409424488991888</v>
       </c>
-      <c r="K9" t="n">
+      <c r="M9" t="n">
         <v>0.409424488991888</v>
       </c>
     </row>
@@ -788,12 +842,18 @@
         <v>0.252114892247038</v>
       </c>
       <c r="I10" t="n">
+        <v>0.07007962478060897</v>
+      </c>
+      <c r="J10" t="n">
         <v>-1.274203850807555</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
+        <v>1.274203850807555</v>
+      </c>
+      <c r="L10" t="n">
         <v>-0.8026607538802666</v>
       </c>
-      <c r="K10" t="n">
+      <c r="M10" t="n">
         <v>0.8026607538802666</v>
       </c>
     </row>
@@ -823,12 +883,18 @@
         <v>0.2284968634682203</v>
       </c>
       <c r="I11" t="n">
+        <v>0.03719083035979676</v>
+      </c>
+      <c r="J11" t="n">
         <v>-1.162319534099067</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
+        <v>1.162319534099067</v>
+      </c>
+      <c r="L11" t="n">
         <v>-0.3852978441064636</v>
       </c>
-      <c r="K11" t="n">
+      <c r="M11" t="n">
         <v>0.3852978441064636</v>
       </c>
     </row>
@@ -858,12 +924,18 @@
         <v>0.1191311720564966</v>
       </c>
       <c r="I12" t="n">
+        <v>0.03619552273593946</v>
+      </c>
+      <c r="J12" t="n">
         <v>0.3442443842321475</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
+        <v>0.3442443842321475</v>
+      </c>
+      <c r="L12" t="n">
         <v>0.1115874013155464</v>
       </c>
-      <c r="K12" t="n">
+      <c r="M12" t="n">
         <v>0.1115874013155464</v>
       </c>
     </row>
@@ -893,12 +965,18 @@
         <v>0.1121078194980673</v>
       </c>
       <c r="I13" t="n">
+        <v>0.03801145000663797</v>
+      </c>
+      <c r="J13" t="n">
         <v>0.2886938913263584</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
+        <v>0.2886938913263584</v>
+      </c>
+      <c r="L13" t="n">
         <v>0.1003260225251926</v>
       </c>
-      <c r="K13" t="n">
+      <c r="M13" t="n">
         <v>0.1003260225251926</v>
       </c>
     </row>
@@ -928,12 +1006,18 @@
         <v>0.1045701867003553</v>
       </c>
       <c r="I14" t="n">
+        <v>-0.06954913092679149</v>
+      </c>
+      <c r="J14" t="n">
         <v>0.2305471595849802</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
+        <v>0.2305471595849802</v>
+      </c>
+      <c r="L14" t="n">
         <v>-0.1300404631645038</v>
       </c>
-      <c r="K14" t="n">
+      <c r="M14" t="n">
         <v>0.1300404631645038</v>
       </c>
     </row>
@@ -963,12 +1047,18 @@
         <v>0.09504732941141796</v>
       </c>
       <c r="I15" t="n">
+        <v>-0.01970310092027705</v>
+      </c>
+      <c r="J15" t="n">
         <v>0.1802583930214906</v>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
+        <v>0.1802583930214906</v>
+      </c>
+      <c r="L15" t="n">
         <v>-0.04301075277419363</v>
       </c>
-      <c r="K15" t="n">
+      <c r="M15" t="n">
         <v>0.04301075277419363</v>
       </c>
     </row>
@@ -998,12 +1088,18 @@
         <v>0.09130198016224032</v>
       </c>
       <c r="I16" t="n">
+        <v>-0.006451635241295772</v>
+      </c>
+      <c r="J16" t="n">
         <v>0.1596327558122316</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
+        <v>0.1596327558122316</v>
+      </c>
+      <c r="L16" t="n">
         <v>-0.01043092763543897</v>
       </c>
-      <c r="K16" t="n">
+      <c r="M16" t="n">
         <v>0.01043092763543897</v>
       </c>
     </row>
@@ -1033,12 +1129,18 @@
         <v>0.09324517427804631</v>
       </c>
       <c r="I17" t="n">
+        <v>0.1810127751752835</v>
+      </c>
+      <c r="J17" t="n">
         <v>0.1650565328603363</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
+        <v>0.1650565328603363</v>
+      </c>
+      <c r="L17" t="n">
         <v>0.2264813926689029</v>
       </c>
-      <c r="K17" t="n">
+      <c r="M17" t="n">
         <v>0.2264813926689029</v>
       </c>
     </row>
@@ -1068,12 +1170,18 @@
         <v>0.09150738473624677</v>
       </c>
       <c r="I18" t="n">
+        <v>-0.02883454103336998</v>
+      </c>
+      <c r="J18" t="n">
         <v>0.1537079804978188</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
+        <v>0.1537079804978188</v>
+      </c>
+      <c r="L18" t="n">
         <v>-0.03383659910054636</v>
       </c>
-      <c r="K18" t="n">
+      <c r="M18" t="n">
         <v>0.03383659910054636</v>
       </c>
     </row>
@@ -1103,12 +1211,18 @@
         <v>0.09535303574600616</v>
       </c>
       <c r="I19" t="n">
+        <v>0.1444724872797511</v>
+      </c>
+      <c r="J19" t="n">
         <v>0.187037036984127</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
+        <v>0.187037036984127</v>
+      </c>
+      <c r="L19" t="n">
         <v>0.4024322826344469</v>
       </c>
-      <c r="K19" t="n">
+      <c r="M19" t="n">
         <v>0.4024322826344469</v>
       </c>
     </row>
@@ -1138,12 +1252,18 @@
         <v>0.09308901853300794</v>
       </c>
       <c r="I20" t="n">
+        <v>0.02448929697916169</v>
+      </c>
+      <c r="J20" t="n">
         <v>0.1848466320697034</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
+        <v>0.1848466320697034</v>
+      </c>
+      <c r="L20" t="n">
         <v>0.127823694214876</v>
       </c>
-      <c r="K20" t="n">
+      <c r="M20" t="n">
         <v>0.127823694214876</v>
       </c>
     </row>
@@ -1162,9 +1282,13 @@
       <c r="H21" t="n">
         <v>0.07943046883992988</v>
       </c>
-      <c r="I21" t="inlineStr"/>
+      <c r="I21" t="n">
+        <v>0.0387149826119924</v>
+      </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
comment on Mu, suggestions for parameters, m(gclc) through feed
</commit_message>
<xml_diff>
--- a/data/Yxs_table.xlsx
+++ b/data/Yxs_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,20 +481,30 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>mu 2.1 [1/h]</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>mu 2.2 [1/h]</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>Yxs 1.1 [gx/gs]</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Yxs 1.2 [gx/gs]</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Yxs 2.1 [gx/gs]</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Yxs 2.2 [gx/gs]</t>
         </is>
@@ -528,6 +538,8 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -558,15 +570,19 @@
         <v>0.3346417012349824</v>
       </c>
       <c r="J3" t="n">
-        <v>-14.0151515227274</v>
-      </c>
-      <c r="K3" t="n">
-        <v>14.0151515227274</v>
-      </c>
+        <v>0.3346417012349824</v>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="n">
         <v>-14.0151515227274</v>
       </c>
       <c r="M3" t="n">
+        <v>14.0151515227274</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-14.0151515227274</v>
+      </c>
+      <c r="O3" t="n">
         <v>14.0151515227274</v>
       </c>
     </row>
@@ -599,15 +615,19 @@
         <v>0.8127218063500202</v>
       </c>
       <c r="J4" t="n">
+        <v>0.8127218063500202</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="n">
         <v>-38.54545454545568</v>
       </c>
-      <c r="K4" t="n">
+      <c r="M4" t="n">
         <v>38.54545454545568</v>
       </c>
-      <c r="L4" t="n">
+      <c r="N4" t="n">
         <v>10.51515149999989</v>
       </c>
-      <c r="M4" t="n">
+      <c r="O4" t="n">
         <v>10.51515149999989</v>
       </c>
     </row>
@@ -640,15 +660,19 @@
         <v>0.4243727592997257</v>
       </c>
       <c r="J5" t="n">
+        <v>0.4243727592997257</v>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="n">
         <v>-3.299688472897195</v>
       </c>
-      <c r="K5" t="n">
+      <c r="M5" t="n">
         <v>3.299688472897195</v>
       </c>
-      <c r="L5" t="n">
+      <c r="N5" t="n">
         <v>-1.788174138401557</v>
       </c>
-      <c r="M5" t="n">
+      <c r="O5" t="n">
         <v>1.788174138401557</v>
       </c>
     </row>
@@ -681,15 +705,19 @@
         <v>0.2746536833672744</v>
       </c>
       <c r="J6" t="n">
+        <v>0.2746536833672744</v>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="n">
         <v>-2.568350168686871</v>
       </c>
-      <c r="K6" t="n">
+      <c r="M6" t="n">
         <v>2.568350168686871</v>
       </c>
-      <c r="L6" t="n">
+      <c r="N6" t="n">
         <v>-1.708424909890113</v>
       </c>
-      <c r="M6" t="n">
+      <c r="O6" t="n">
         <v>1.708424909890113</v>
       </c>
     </row>
@@ -722,15 +750,19 @@
         <v>0.1442387591429934</v>
       </c>
       <c r="J7" t="n">
+        <v>0.1442387591429934</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="n">
         <v>-1.73448275862069</v>
       </c>
-      <c r="K7" t="n">
+      <c r="M7" t="n">
         <v>1.73448275862069</v>
       </c>
-      <c r="L7" t="n">
+      <c r="N7" t="n">
         <v>-0.633777777333333</v>
       </c>
-      <c r="M7" t="n">
+      <c r="O7" t="n">
         <v>0.633777777333333</v>
       </c>
     </row>
@@ -763,15 +795,19 @@
         <v>0.2217057364726398</v>
       </c>
       <c r="J8" t="n">
+        <v>0.2217057364726398</v>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="n">
         <v>-1.684195525010689</v>
       </c>
-      <c r="K8" t="n">
+      <c r="M8" t="n">
         <v>1.684195525010689</v>
       </c>
-      <c r="L8" t="n">
+      <c r="N8" t="n">
         <v>-1.538119086811352</v>
       </c>
-      <c r="M8" t="n">
+      <c r="O8" t="n">
         <v>1.538119086811352</v>
       </c>
     </row>
@@ -804,15 +840,19 @@
         <v>0.07735908689312881</v>
       </c>
       <c r="J9" t="n">
+        <v>0.07735908689312881</v>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="n">
         <v>-1.340620445658963</v>
       </c>
-      <c r="K9" t="n">
+      <c r="M9" t="n">
         <v>1.340620445658963</v>
       </c>
-      <c r="L9" t="n">
+      <c r="N9" t="n">
         <v>-0.409424488991888</v>
       </c>
-      <c r="M9" t="n">
+      <c r="O9" t="n">
         <v>0.409424488991888</v>
       </c>
     </row>
@@ -844,16 +884,18 @@
       <c r="I10" t="n">
         <v>0.07007962478060897</v>
       </c>
-      <c r="J10" t="n">
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="n">
         <v>-1.274203850807555</v>
       </c>
-      <c r="K10" t="n">
+      <c r="M10" t="n">
         <v>1.274203850807555</v>
       </c>
-      <c r="L10" t="n">
+      <c r="N10" t="n">
         <v>-0.8026607538802666</v>
       </c>
-      <c r="M10" t="n">
+      <c r="O10" t="n">
         <v>0.8026607538802666</v>
       </c>
     </row>
@@ -885,16 +927,20 @@
       <c r="I11" t="n">
         <v>0.03719083035979676</v>
       </c>
-      <c r="J11" t="n">
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="n">
+        <v>0.03719083035979676</v>
+      </c>
+      <c r="L11" t="n">
         <v>-1.162319534099067</v>
       </c>
-      <c r="K11" t="n">
+      <c r="M11" t="n">
         <v>1.162319534099067</v>
       </c>
-      <c r="L11" t="n">
+      <c r="N11" t="n">
         <v>-0.3852978441064636</v>
       </c>
-      <c r="M11" t="n">
+      <c r="O11" t="n">
         <v>0.3852978441064636</v>
       </c>
     </row>
@@ -926,16 +972,20 @@
       <c r="I12" t="n">
         <v>0.03619552273593946</v>
       </c>
-      <c r="J12" t="n">
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="n">
+        <v>0.03619552273593946</v>
+      </c>
+      <c r="L12" t="n">
         <v>0.3442443842321475</v>
       </c>
-      <c r="K12" t="n">
+      <c r="M12" t="n">
         <v>0.3442443842321475</v>
       </c>
-      <c r="L12" t="n">
+      <c r="N12" t="n">
         <v>0.1115874013155464</v>
       </c>
-      <c r="M12" t="n">
+      <c r="O12" t="n">
         <v>0.1115874013155464</v>
       </c>
     </row>
@@ -967,16 +1017,20 @@
       <c r="I13" t="n">
         <v>0.03801145000663797</v>
       </c>
-      <c r="J13" t="n">
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="n">
+        <v>0.03801145000663797</v>
+      </c>
+      <c r="L13" t="n">
         <v>0.2886938913263584</v>
       </c>
-      <c r="K13" t="n">
+      <c r="M13" t="n">
         <v>0.2886938913263584</v>
       </c>
-      <c r="L13" t="n">
+      <c r="N13" t="n">
         <v>0.1003260225251926</v>
       </c>
-      <c r="M13" t="n">
+      <c r="O13" t="n">
         <v>0.1003260225251926</v>
       </c>
     </row>
@@ -1008,16 +1062,20 @@
       <c r="I14" t="n">
         <v>-0.06954913092679149</v>
       </c>
-      <c r="J14" t="n">
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="n">
+        <v>-0.06954913092679149</v>
+      </c>
+      <c r="L14" t="n">
         <v>0.2305471595849802</v>
       </c>
-      <c r="K14" t="n">
+      <c r="M14" t="n">
         <v>0.2305471595849802</v>
       </c>
-      <c r="L14" t="n">
+      <c r="N14" t="n">
         <v>-0.1300404631645038</v>
       </c>
-      <c r="M14" t="n">
+      <c r="O14" t="n">
         <v>0.1300404631645038</v>
       </c>
     </row>
@@ -1049,16 +1107,20 @@
       <c r="I15" t="n">
         <v>-0.01970310092027705</v>
       </c>
-      <c r="J15" t="n">
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="n">
+        <v>-0.01970310092027705</v>
+      </c>
+      <c r="L15" t="n">
         <v>0.1802583930214906</v>
       </c>
-      <c r="K15" t="n">
+      <c r="M15" t="n">
         <v>0.1802583930214906</v>
       </c>
-      <c r="L15" t="n">
+      <c r="N15" t="n">
         <v>-0.04301075277419363</v>
       </c>
-      <c r="M15" t="n">
+      <c r="O15" t="n">
         <v>0.04301075277419363</v>
       </c>
     </row>
@@ -1090,16 +1152,20 @@
       <c r="I16" t="n">
         <v>-0.006451635241295772</v>
       </c>
-      <c r="J16" t="n">
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="n">
+        <v>-0.006451635241295772</v>
+      </c>
+      <c r="L16" t="n">
         <v>0.1596327558122316</v>
       </c>
-      <c r="K16" t="n">
+      <c r="M16" t="n">
         <v>0.1596327558122316</v>
       </c>
-      <c r="L16" t="n">
+      <c r="N16" t="n">
         <v>-0.01043092763543897</v>
       </c>
-      <c r="M16" t="n">
+      <c r="O16" t="n">
         <v>0.01043092763543897</v>
       </c>
     </row>
@@ -1131,16 +1197,20 @@
       <c r="I17" t="n">
         <v>0.1810127751752835</v>
       </c>
-      <c r="J17" t="n">
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="n">
+        <v>0.1810127751752835</v>
+      </c>
+      <c r="L17" t="n">
         <v>0.1650565328603363</v>
       </c>
-      <c r="K17" t="n">
+      <c r="M17" t="n">
         <v>0.1650565328603363</v>
       </c>
-      <c r="L17" t="n">
+      <c r="N17" t="n">
         <v>0.2264813926689029</v>
       </c>
-      <c r="M17" t="n">
+      <c r="O17" t="n">
         <v>0.2264813926689029</v>
       </c>
     </row>
@@ -1172,16 +1242,20 @@
       <c r="I18" t="n">
         <v>-0.02883454103336998</v>
       </c>
-      <c r="J18" t="n">
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="n">
+        <v>-0.02883454103336998</v>
+      </c>
+      <c r="L18" t="n">
         <v>0.1537079804978188</v>
       </c>
-      <c r="K18" t="n">
+      <c r="M18" t="n">
         <v>0.1537079804978188</v>
       </c>
-      <c r="L18" t="n">
+      <c r="N18" t="n">
         <v>-0.03383659910054636</v>
       </c>
-      <c r="M18" t="n">
+      <c r="O18" t="n">
         <v>0.03383659910054636</v>
       </c>
     </row>
@@ -1213,16 +1287,20 @@
       <c r="I19" t="n">
         <v>0.1444724872797511</v>
       </c>
-      <c r="J19" t="n">
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="n">
+        <v>0.1444724872797511</v>
+      </c>
+      <c r="L19" t="n">
         <v>0.187037036984127</v>
       </c>
-      <c r="K19" t="n">
+      <c r="M19" t="n">
         <v>0.187037036984127</v>
       </c>
-      <c r="L19" t="n">
+      <c r="N19" t="n">
         <v>0.4024322826344469</v>
       </c>
-      <c r="M19" t="n">
+      <c r="O19" t="n">
         <v>0.4024322826344469</v>
       </c>
     </row>
@@ -1254,16 +1332,20 @@
       <c r="I20" t="n">
         <v>0.02448929697916169</v>
       </c>
-      <c r="J20" t="n">
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="n">
+        <v>0.02448929697916169</v>
+      </c>
+      <c r="L20" t="n">
         <v>0.1848466320697034</v>
       </c>
-      <c r="K20" t="n">
+      <c r="M20" t="n">
         <v>0.1848466320697034</v>
       </c>
-      <c r="L20" t="n">
+      <c r="N20" t="n">
         <v>0.127823694214876</v>
       </c>
-      <c r="M20" t="n">
+      <c r="O20" t="n">
         <v>0.127823694214876</v>
       </c>
     </row>
@@ -1286,9 +1368,13 @@
         <v>0.0387149826119924</v>
       </c>
       <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
+      <c r="K21" t="n">
+        <v>0.0387149826119924</v>
+      </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Mu, Yxs and qs
</commit_message>
<xml_diff>
--- a/data/Yxs_table.xlsx
+++ b/data/Yxs_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,42 +471,47 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>mu 1 [1/h]</t>
+          <t>Glucose2 [g/L]</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>mu 2 [1/h]</t>
+          <t>Glucose [g/L].1</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>mu 2.1 [1/h]</t>
+          <t>added Glucose  [g]</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>mu 2.2 [1/h]</t>
+          <t>Consumed_Glucose [g]</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Yxs 1.1 [gx/gs]</t>
+          <t>Consumed_Glucose [g/L]</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Yxs 1.2 [gx/gs]</t>
+          <t>Volume at each time point</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Yxs 2.1 [gx/gs]</t>
+          <t>mu between direct samples [1/h]</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Yxs 2.2 [gx/gs]</t>
+          <t>Yxs [gx/gs]</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>qs 1 - ds/dt/x - [1/h]</t>
         </is>
       </c>
     </row>
@@ -518,7 +523,7 @@
         <v>0.2</v>
       </c>
       <c r="C2" t="n">
-        <v>5.22</v>
+        <v>10.44</v>
       </c>
       <c r="D2" t="n">
         <v>0.167</v>
@@ -532,14 +537,27 @@
       <c r="G2" t="n">
         <v>0.079</v>
       </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="I2" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="J2" t="n">
+        <v>10.44</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -549,7 +567,7 @@
         <v>2.1</v>
       </c>
       <c r="C3" t="n">
-        <v>5.176</v>
+        <v>10.352</v>
       </c>
       <c r="D3" t="n">
         <v>0.16</v>
@@ -564,26 +582,31 @@
         <v>0.104</v>
       </c>
       <c r="H3" t="n">
-        <v>0.3346417012349824</v>
+        <v>5.176</v>
       </c>
       <c r="I3" t="n">
-        <v>0.3346417012349824</v>
+        <v>5.176</v>
       </c>
       <c r="J3" t="n">
-        <v>0.3346417012349824</v>
-      </c>
-      <c r="K3" t="inlineStr"/>
+        <v>10.44</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.08799999999999911</v>
+      </c>
       <c r="L3" t="n">
-        <v>-14.0151515227274</v>
+        <v>0.08799999999999911</v>
       </c>
       <c r="M3" t="n">
-        <v>14.0151515227274</v>
+        <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>-14.0151515227274</v>
+        <v>0.4676677286516002</v>
       </c>
       <c r="O3" t="n">
-        <v>14.0151515227274</v>
+        <v>7.007575761363708</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.06673744880934256</v>
       </c>
     </row>
     <row r="4">
@@ -594,7 +617,7 @@
         <v>2.3</v>
       </c>
       <c r="C4" t="n">
-        <v>5.198</v>
+        <v>10.396</v>
       </c>
       <c r="D4" t="n">
         <v>0.118</v>
@@ -609,26 +632,31 @@
         <v>0.334</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3801731398173669</v>
+        <v>5.198</v>
       </c>
       <c r="I4" t="n">
-        <v>0.8127218063500202</v>
+        <v>5.198</v>
       </c>
       <c r="J4" t="n">
-        <v>0.8127218063500202</v>
-      </c>
-      <c r="K4" t="inlineStr"/>
+        <v>10.44</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.0439999999999987</v>
+      </c>
       <c r="L4" t="n">
-        <v>-38.54545454545568</v>
+        <v>0.0439999999999987</v>
       </c>
       <c r="M4" t="n">
-        <v>38.54545454545568</v>
+        <v>1</v>
       </c>
       <c r="N4" t="n">
-        <v>10.51515149999989</v>
+        <v>0.8825025417389376</v>
       </c>
       <c r="O4" t="n">
-        <v>10.51515149999989</v>
+        <v>5.257575749999952</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.1678535096216057</v>
       </c>
     </row>
     <row r="5">
@@ -639,7 +667,7 @@
         <v>3.4</v>
       </c>
       <c r="C5" t="n">
-        <v>4.685</v>
+        <v>9.369999999999999</v>
       </c>
       <c r="D5" t="n">
         <v>0.141</v>
@@ -654,26 +682,31 @@
         <v>0.357</v>
       </c>
       <c r="H5" t="n">
-        <v>0.3953667590144278</v>
+        <v>4.685</v>
       </c>
       <c r="I5" t="n">
-        <v>0.4243727592997257</v>
+        <v>4.685</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4243727592997257</v>
-      </c>
-      <c r="K5" t="inlineStr"/>
+        <v>10.44</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1.070000000000001</v>
+      </c>
       <c r="L5" t="n">
-        <v>-3.299688472897195</v>
+        <v>1.070000000000001</v>
       </c>
       <c r="M5" t="n">
-        <v>3.299688472897195</v>
+        <v>1</v>
       </c>
       <c r="N5" t="n">
-        <v>-1.788174138401557</v>
+        <v>0.5408167273906378</v>
       </c>
       <c r="O5" t="n">
-        <v>1.788174138401557</v>
+        <v>0.8940870692007782</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.6048814998231351</v>
       </c>
     </row>
     <row r="6">
@@ -684,7 +717,7 @@
         <v>4.4</v>
       </c>
       <c r="C6" t="n">
-        <v>4.23</v>
+        <v>8.460000000000001</v>
       </c>
       <c r="D6" t="n">
         <v>0.187</v>
@@ -699,26 +732,31 @@
         <v>0.148</v>
       </c>
       <c r="H6" t="n">
-        <v>0.3666255505270102</v>
+        <v>4.23</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2746536833672744</v>
+        <v>4.23</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2746536833672744</v>
-      </c>
-      <c r="K6" t="inlineStr"/>
+        <v>10.44</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1.979999999999998</v>
+      </c>
       <c r="L6" t="n">
-        <v>-2.568350168686871</v>
+        <v>1.979999999999998</v>
       </c>
       <c r="M6" t="n">
-        <v>2.568350168686871</v>
+        <v>1</v>
       </c>
       <c r="N6" t="n">
-        <v>-1.708424909890113</v>
+        <v>0.3160748173374999</v>
       </c>
       <c r="O6" t="n">
-        <v>1.708424909890113</v>
+        <v>0.854212454945057</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.370018975382219</v>
       </c>
     </row>
     <row r="7">
@@ -729,7 +767,7 @@
         <v>5.35</v>
       </c>
       <c r="C7" t="n">
-        <v>3.48</v>
+        <v>6.96</v>
       </c>
       <c r="D7" t="n">
         <v>0.21</v>
@@ -744,26 +782,31 @@
         <v>0.146</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3256027443493761</v>
+        <v>3.48</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1442387591429934</v>
+        <v>3.48</v>
       </c>
       <c r="J7" t="n">
-        <v>0.1442387591429934</v>
-      </c>
-      <c r="K7" t="inlineStr"/>
+        <v>10.44</v>
+      </c>
+      <c r="K7" t="n">
+        <v>3.48</v>
+      </c>
       <c r="L7" t="n">
-        <v>-1.73448275862069</v>
+        <v>3.48</v>
       </c>
       <c r="M7" t="n">
-        <v>1.73448275862069</v>
+        <v>1</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.633777777333333</v>
+        <v>0.15458832444611</v>
       </c>
       <c r="O7" t="n">
-        <v>0.633777777333333</v>
+        <v>0.3168888886666664</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.4878313187204257</v>
       </c>
     </row>
     <row r="8">
@@ -774,7 +817,7 @@
         <v>6.35</v>
       </c>
       <c r="C8" t="n">
-        <v>2.881</v>
+        <v>5.762</v>
       </c>
       <c r="D8" t="n">
         <v>0.276</v>
@@ -789,26 +832,31 @@
         <v>0.128</v>
       </c>
       <c r="H8" t="n">
-        <v>0.3087089219303946</v>
+        <v>2.881</v>
       </c>
       <c r="I8" t="n">
-        <v>0.2217057364726398</v>
+        <v>2.881</v>
       </c>
       <c r="J8" t="n">
-        <v>0.2217057364726398</v>
-      </c>
-      <c r="K8" t="inlineStr"/>
+        <v>10.44</v>
+      </c>
+      <c r="K8" t="n">
+        <v>4.678</v>
+      </c>
       <c r="L8" t="n">
-        <v>-1.684195525010689</v>
+        <v>4.678</v>
       </c>
       <c r="M8" t="n">
-        <v>1.684195525010689</v>
+        <v>1</v>
       </c>
       <c r="N8" t="n">
-        <v>-1.538119086811352</v>
+        <v>0.2482040228987069</v>
       </c>
       <c r="O8" t="n">
-        <v>1.538119086811352</v>
+        <v>0.7690595434056761</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.3227370689655173</v>
       </c>
     </row>
     <row r="9">
@@ -819,7 +867,7 @@
         <v>7.3</v>
       </c>
       <c r="C9" t="n">
-        <v>2.018</v>
+        <v>4.036</v>
       </c>
       <c r="D9" t="n">
         <v>0.381</v>
@@ -834,26 +882,31 @@
         <v>0.141</v>
       </c>
       <c r="H9" t="n">
-        <v>0.2777536623127322</v>
+        <v>2.018</v>
       </c>
       <c r="I9" t="n">
-        <v>0.07735908689312881</v>
+        <v>2.018</v>
       </c>
       <c r="J9" t="n">
-        <v>0.07735908689312881</v>
-      </c>
-      <c r="K9" t="inlineStr"/>
+        <v>10.44</v>
+      </c>
+      <c r="K9" t="n">
+        <v>6.404</v>
+      </c>
       <c r="L9" t="n">
-        <v>-1.340620445658963</v>
+        <v>6.404</v>
       </c>
       <c r="M9" t="n">
-        <v>1.340620445658963</v>
+        <v>1</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.409424488991888</v>
+        <v>0.08027262416329092</v>
       </c>
       <c r="O9" t="n">
-        <v>0.409424488991888</v>
+        <v>0.204712244495944</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.3921241954087479</v>
       </c>
     </row>
     <row r="10">
@@ -864,7 +917,7 @@
         <v>8.300000000000001</v>
       </c>
       <c r="C10" t="n">
-        <v>1.567</v>
+        <v>3.134</v>
       </c>
       <c r="D10" t="n">
         <v>0.467</v>
@@ -879,24 +932,31 @@
         <v>0.1</v>
       </c>
       <c r="H10" t="n">
-        <v>0.252114892247038</v>
+        <v>1.567</v>
       </c>
       <c r="I10" t="n">
-        <v>0.07007962478060897</v>
-      </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+        <v>1.567</v>
+      </c>
+      <c r="J10" t="n">
+        <v>10.44</v>
+      </c>
+      <c r="K10" t="n">
+        <v>7.305999999999999</v>
+      </c>
       <c r="L10" t="n">
-        <v>-1.274203850807555</v>
+        <v>7.305999999999999</v>
       </c>
       <c r="M10" t="n">
-        <v>1.274203850807555</v>
+        <v>1</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.8026607538802666</v>
+        <v>0.07259358288284798</v>
       </c>
       <c r="O10" t="n">
-        <v>0.8026607538802666</v>
+        <v>0.4013303769401335</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.1808823529290851</v>
       </c>
     </row>
     <row r="11">
@@ -907,7 +967,7 @@
         <v>9.300000000000001</v>
       </c>
       <c r="C11" t="n">
-        <v>1.041</v>
+        <v>2.082</v>
       </c>
       <c r="D11" t="n">
         <v>0.429</v>
@@ -922,26 +982,31 @@
         <v>0.156</v>
       </c>
       <c r="H11" t="n">
-        <v>0.2284968634682203</v>
+        <v>1.041</v>
       </c>
       <c r="I11" t="n">
-        <v>0.03719083035979676</v>
-      </c>
-      <c r="J11" t="inlineStr"/>
+        <v>1.041</v>
+      </c>
+      <c r="J11" t="n">
+        <v>10.44</v>
+      </c>
       <c r="K11" t="n">
-        <v>0.03719083035979676</v>
+        <v>8.358000000000001</v>
       </c>
       <c r="L11" t="n">
-        <v>-1.162319534099067</v>
+        <v>8.358000000000001</v>
       </c>
       <c r="M11" t="n">
-        <v>1.162319534099067</v>
+        <v>1</v>
       </c>
       <c r="N11" t="n">
-        <v>-0.3852978441064636</v>
+        <v>0.03789106306631612</v>
       </c>
       <c r="O11" t="n">
-        <v>0.3852978441064636</v>
+        <v>0.1926489220532315</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.1966845319583273</v>
       </c>
     </row>
     <row r="12">
@@ -952,7 +1017,7 @@
         <v>21.3</v>
       </c>
       <c r="C12" t="n">
-        <v>28.102</v>
+        <v>56.204</v>
       </c>
       <c r="D12" t="n">
         <v>1.489</v>
@@ -967,26 +1032,31 @@
         <v>0.058</v>
       </c>
       <c r="H12" t="n">
-        <v>0.1191311720564966</v>
+        <v>28.102</v>
       </c>
       <c r="I12" t="n">
-        <v>0.03619552273593946</v>
-      </c>
-      <c r="J12" t="inlineStr"/>
+        <v>28.102</v>
+      </c>
+      <c r="J12" t="n">
+        <v>145.862</v>
+      </c>
       <c r="K12" t="n">
-        <v>0.03619552273593946</v>
+        <v>89.65799999999999</v>
       </c>
       <c r="L12" t="n">
-        <v>0.3442443842321475</v>
+        <v>68.74173270281385</v>
       </c>
       <c r="M12" t="n">
-        <v>0.3442443842321475</v>
+        <v>1.304273204570096</v>
       </c>
       <c r="N12" t="n">
-        <v>0.1115874013155464</v>
+        <v>0.04532945039001619</v>
       </c>
       <c r="O12" t="n">
-        <v>0.1115874013155464</v>
+        <v>0.0500079496883982</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.9064448887120156</v>
       </c>
     </row>
     <row r="13">
@@ -997,7 +1067,7 @@
         <v>23.3</v>
       </c>
       <c r="C13" t="n">
-        <v>34.85</v>
+        <v>69.7</v>
       </c>
       <c r="D13" t="n">
         <v>1.45</v>
@@ -1012,26 +1082,31 @@
         <v>0.048</v>
       </c>
       <c r="H13" t="n">
-        <v>0.1121078194980673</v>
+        <v>34.85</v>
       </c>
       <c r="I13" t="n">
-        <v>0.03801145000663797</v>
-      </c>
-      <c r="J13" t="inlineStr"/>
+        <v>34.85</v>
+      </c>
+      <c r="J13" t="n">
+        <v>169.662</v>
+      </c>
       <c r="K13" t="n">
-        <v>0.03801145000663797</v>
+        <v>99.962</v>
       </c>
       <c r="L13" t="n">
-        <v>0.2886938913263584</v>
+        <v>71.68328608621864</v>
       </c>
       <c r="M13" t="n">
-        <v>0.2886938913263584</v>
+        <v>1.394495222774365</v>
       </c>
       <c r="N13" t="n">
-        <v>0.1003260225251926</v>
+        <v>0.03949364134873408</v>
       </c>
       <c r="O13" t="n">
-        <v>0.1003260225251926</v>
+        <v>0.2301505061303305</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.1715991939916459</v>
       </c>
     </row>
     <row r="14">
@@ -1042,7 +1117,7 @@
         <v>24.3</v>
       </c>
       <c r="C14" t="n">
-        <v>39.628</v>
+        <v>79.256</v>
       </c>
       <c r="D14" t="n">
         <v>1.49</v>
@@ -1057,26 +1132,31 @@
         <v>0.031</v>
       </c>
       <c r="H14" t="n">
-        <v>0.1045701867003553</v>
+        <v>39.628</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.06954913092679149</v>
-      </c>
-      <c r="J14" t="inlineStr"/>
+        <v>39.628</v>
+      </c>
+      <c r="J14" t="n">
+        <v>181.562</v>
+      </c>
       <c r="K14" t="n">
-        <v>-0.06954913092679149</v>
+        <v>102.306</v>
       </c>
       <c r="L14" t="n">
-        <v>0.2305471595849802</v>
+        <v>70.83332697721671</v>
       </c>
       <c r="M14" t="n">
-        <v>0.2305471595849802</v>
+        <v>1.444320129603772</v>
       </c>
       <c r="N14" t="n">
-        <v>-0.1300404631645038</v>
+        <v>0.06718569777249125</v>
       </c>
       <c r="O14" t="n">
-        <v>0.1300404631645038</v>
+        <v>0.7310155587715322</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.09190734310141971</v>
       </c>
     </row>
     <row r="15">
@@ -1087,7 +1167,7 @@
         <v>26.3</v>
       </c>
       <c r="C15" t="n">
-        <v>47.378</v>
+        <v>94.756</v>
       </c>
       <c r="D15" t="n">
         <v>1.431</v>
@@ -1102,26 +1182,31 @@
         <v>0.025</v>
       </c>
       <c r="H15" t="n">
-        <v>0.09504732941141796</v>
+        <v>47.378</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.01970310092027705</v>
-      </c>
-      <c r="J15" t="inlineStr"/>
+        <v>47.378</v>
+      </c>
+      <c r="J15" t="n">
+        <v>205.362</v>
+      </c>
       <c r="K15" t="n">
-        <v>-0.01970310092027705</v>
+        <v>110.606</v>
       </c>
       <c r="L15" t="n">
-        <v>0.1802583930214906</v>
+        <v>71.18688537354446</v>
       </c>
       <c r="M15" t="n">
-        <v>0.1802583930214906</v>
+        <v>1.553741246292889</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.04301075277419363</v>
+        <v>0.01931993821409123</v>
       </c>
       <c r="O15" t="n">
-        <v>0.04301075277419363</v>
+        <v>0.9427956950314005</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.02049217907539105</v>
       </c>
     </row>
     <row r="16">
@@ -1132,7 +1217,7 @@
         <v>27.3</v>
       </c>
       <c r="C16" t="n">
-        <v>52.491</v>
+        <v>104.982</v>
       </c>
       <c r="D16" t="n">
         <v>1.394</v>
@@ -1147,26 +1232,31 @@
         <v>0.153</v>
       </c>
       <c r="H16" t="n">
-        <v>0.09130198016224032</v>
+        <v>52.491</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.006451635241295772</v>
-      </c>
-      <c r="J16" t="inlineStr"/>
+        <v>52.491</v>
+      </c>
+      <c r="J16" t="n">
+        <v>217.262</v>
+      </c>
       <c r="K16" t="n">
-        <v>-0.006451635241295772</v>
+        <v>112.28</v>
       </c>
       <c r="L16" t="n">
-        <v>0.1596327558122316</v>
+        <v>69.55804999721735</v>
       </c>
       <c r="M16" t="n">
-        <v>0.1596327558122316</v>
+        <v>1.614191312213205</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.01043092763543897</v>
+        <v>0.006430868127268053</v>
       </c>
       <c r="O16" t="n">
-        <v>0.01043092763543897</v>
+        <v>0.03274323100733601</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.1964029794685576</v>
       </c>
     </row>
     <row r="17">
@@ -1177,7 +1267,7 @@
         <v>27.9</v>
       </c>
       <c r="C17" t="n">
-        <v>56.665</v>
+        <v>113.33</v>
       </c>
       <c r="D17" t="n">
         <v>1.214</v>
@@ -1192,26 +1282,31 @@
         <v>0.204</v>
       </c>
       <c r="H17" t="n">
-        <v>0.09324517427804631</v>
+        <v>56.665</v>
       </c>
       <c r="I17" t="n">
-        <v>0.1810127751752835</v>
-      </c>
-      <c r="J17" t="inlineStr"/>
+        <v>56.665</v>
+      </c>
+      <c r="J17" t="n">
+        <v>224.402</v>
+      </c>
       <c r="K17" t="n">
-        <v>0.1810127751752835</v>
+        <v>111.072</v>
       </c>
       <c r="L17" t="n">
-        <v>0.1650565328603363</v>
+        <v>67.20575159889712</v>
       </c>
       <c r="M17" t="n">
-        <v>0.1650565328603363</v>
+        <v>1.652715688129031</v>
       </c>
       <c r="N17" t="n">
-        <v>0.2264813926689029</v>
+        <v>0.1912081984223309</v>
       </c>
       <c r="O17" t="n">
-        <v>0.2264813926689029</v>
+        <v>0.4018764514209001</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.4757885109871031</v>
       </c>
     </row>
     <row r="18">
@@ -1222,7 +1317,7 @@
         <v>28.3</v>
       </c>
       <c r="C18" t="n">
-        <v>59.778</v>
+        <v>119.556</v>
       </c>
       <c r="D18" t="n">
         <v>0.9379999999999999</v>
@@ -1237,26 +1332,31 @@
         <v>0.06900000000000001</v>
       </c>
       <c r="H18" t="n">
-        <v>0.09150738473624677</v>
+        <v>59.778</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.02883454103336998</v>
-      </c>
-      <c r="J18" t="inlineStr"/>
+        <v>59.778</v>
+      </c>
+      <c r="J18" t="n">
+        <v>236.3</v>
+      </c>
       <c r="K18" t="n">
-        <v>-0.02883454103336998</v>
+        <v>116.744</v>
       </c>
       <c r="L18" t="n">
-        <v>0.1537079804978188</v>
+        <v>69.04709955852459</v>
       </c>
       <c r="M18" t="n">
-        <v>0.1537079804978188</v>
+        <v>1.690787893285037</v>
       </c>
       <c r="N18" t="n">
-        <v>-0.03383659910054636</v>
+        <v>0.02866889234753486</v>
       </c>
       <c r="O18" t="n">
-        <v>0.03383659910054636</v>
+        <v>0.05720446939388425</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.5011652524933631</v>
       </c>
     </row>
     <row r="19">
@@ -1267,7 +1367,7 @@
         <v>30.5</v>
       </c>
       <c r="C19" t="n">
-        <v>68.22</v>
+        <v>136.44</v>
       </c>
       <c r="D19" t="n">
         <v>0.163</v>
@@ -1282,26 +1382,31 @@
         <v>0.041</v>
       </c>
       <c r="H19" t="n">
-        <v>0.09535303574600616</v>
+        <v>150.34</v>
       </c>
       <c r="I19" t="n">
-        <v>0.1444724872797511</v>
-      </c>
-      <c r="J19" t="inlineStr"/>
+        <v>68.22</v>
+      </c>
+      <c r="J19" t="n">
+        <v>314.84</v>
+      </c>
       <c r="K19" t="n">
-        <v>0.1444724872797511</v>
+        <v>178.4</v>
       </c>
       <c r="L19" t="n">
-        <v>0.187037036984127</v>
+        <v>90.54990952549136</v>
       </c>
       <c r="M19" t="n">
-        <v>0.187037036984127</v>
+        <v>1.970184188309733</v>
       </c>
       <c r="N19" t="n">
-        <v>0.4024322826344469</v>
+        <v>0.1700707514016821</v>
       </c>
       <c r="O19" t="n">
-        <v>0.4024322826344469</v>
+        <v>0.1579948544036376</v>
+      </c>
+      <c r="P19" t="n">
+        <v>1.076432217008749</v>
       </c>
     </row>
     <row r="20">
@@ -1312,7 +1417,7 @@
         <v>31.5</v>
       </c>
       <c r="C20" t="n">
-        <v>70.64</v>
+        <v>141.28</v>
       </c>
       <c r="D20" t="n">
         <v>0.038</v>
@@ -1327,26 +1432,31 @@
         <v>0.122</v>
       </c>
       <c r="H20" t="n">
-        <v>0.09308901853300794</v>
+        <v>170.96</v>
       </c>
       <c r="I20" t="n">
-        <v>0.02448929697916169</v>
-      </c>
-      <c r="J20" t="inlineStr"/>
+        <v>70.64</v>
+      </c>
+      <c r="J20" t="n">
+        <v>350.84</v>
+      </c>
       <c r="K20" t="n">
-        <v>0.02448929697916169</v>
+        <v>209.56</v>
       </c>
       <c r="L20" t="n">
-        <v>0.1848466320697034</v>
+        <v>99.5918914827856</v>
       </c>
       <c r="M20" t="n">
-        <v>0.1848466320697034</v>
+        <v>2.104187367866412</v>
       </c>
       <c r="N20" t="n">
-        <v>0.127823694214876</v>
+        <v>0.02479162268240855</v>
       </c>
       <c r="O20" t="n">
-        <v>0.127823694214876</v>
+        <v>0.03421078934474742</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.7246726298121779</v>
       </c>
     </row>
     <row r="21">
@@ -1356,25 +1466,38 @@
       <c r="B21" t="n">
         <v>42</v>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="n">
+        <v>120.475</v>
+      </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
-        <v>0.07943046883992988</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0.0387149826119924</v>
-      </c>
-      <c r="J21" t="inlineStr"/>
+        <v>120.475</v>
+      </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="n">
+        <v>360.44</v>
+      </c>
       <c r="K21" t="n">
-        <v>0.0387149826119924</v>
-      </c>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
+        <v>239.965</v>
+      </c>
+      <c r="L21" t="n">
+        <v>98.09957483368598</v>
+      </c>
+      <c r="M21" t="n">
+        <v>2.446137003211552</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.0477680122771348</v>
+      </c>
+      <c r="O21" t="n">
+        <v>4.297568705589018</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.01111512474832855</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
tried to add dCO2/dt to the model
</commit_message>
<xml_diff>
--- a/data/Yxs_table.xlsx
+++ b/data/Yxs_table.xlsx
@@ -522,9 +522,7 @@
       <c r="B2" t="n">
         <v>0.2</v>
       </c>
-      <c r="C2" t="n">
-        <v>10.44</v>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
         <v>0.167</v>
       </c>
@@ -546,12 +544,8 @@
       <c r="J2" t="n">
         <v>10.44</v>
       </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
         <v>1</v>
       </c>
@@ -566,9 +560,7 @@
       <c r="B3" t="n">
         <v>2.1</v>
       </c>
-      <c r="C3" t="n">
-        <v>10.352</v>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
         <v>0.16</v>
       </c>
@@ -590,24 +582,16 @@
       <c r="J3" t="n">
         <v>10.44</v>
       </c>
-      <c r="K3" t="n">
-        <v>0.08799999999999911</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.08799999999999911</v>
-      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
         <v>1</v>
       </c>
       <c r="N3" t="n">
         <v>0.4676677286516002</v>
       </c>
-      <c r="O3" t="n">
-        <v>7.007575761363708</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0.06673744880934256</v>
-      </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -616,9 +600,7 @@
       <c r="B4" t="n">
         <v>2.3</v>
       </c>
-      <c r="C4" t="n">
-        <v>10.396</v>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
         <v>0.118</v>
       </c>
@@ -640,24 +622,16 @@
       <c r="J4" t="n">
         <v>10.44</v>
       </c>
-      <c r="K4" t="n">
-        <v>0.0439999999999987</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.0439999999999987</v>
-      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
         <v>1</v>
       </c>
       <c r="N4" t="n">
         <v>0.8825025417389376</v>
       </c>
-      <c r="O4" t="n">
-        <v>5.257575749999952</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0.1678535096216057</v>
-      </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -666,9 +640,7 @@
       <c r="B5" t="n">
         <v>3.4</v>
       </c>
-      <c r="C5" t="n">
-        <v>9.369999999999999</v>
-      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
         <v>0.141</v>
       </c>
@@ -690,24 +662,16 @@
       <c r="J5" t="n">
         <v>10.44</v>
       </c>
-      <c r="K5" t="n">
-        <v>1.070000000000001</v>
-      </c>
-      <c r="L5" t="n">
-        <v>1.070000000000001</v>
-      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
         <v>1</v>
       </c>
       <c r="N5" t="n">
         <v>0.5408167273906378</v>
       </c>
-      <c r="O5" t="n">
-        <v>0.8940870692007782</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.6048814998231351</v>
-      </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -716,9 +680,7 @@
       <c r="B6" t="n">
         <v>4.4</v>
       </c>
-      <c r="C6" t="n">
-        <v>8.460000000000001</v>
-      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
         <v>0.187</v>
       </c>
@@ -740,24 +702,16 @@
       <c r="J6" t="n">
         <v>10.44</v>
       </c>
-      <c r="K6" t="n">
-        <v>1.979999999999998</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1.979999999999998</v>
-      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
         <v>1</v>
       </c>
       <c r="N6" t="n">
         <v>0.3160748173374999</v>
       </c>
-      <c r="O6" t="n">
-        <v>0.854212454945057</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.370018975382219</v>
-      </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -766,9 +720,7 @@
       <c r="B7" t="n">
         <v>5.35</v>
       </c>
-      <c r="C7" t="n">
-        <v>6.96</v>
-      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
         <v>0.21</v>
       </c>
@@ -790,24 +742,16 @@
       <c r="J7" t="n">
         <v>10.44</v>
       </c>
-      <c r="K7" t="n">
-        <v>3.48</v>
-      </c>
-      <c r="L7" t="n">
-        <v>3.48</v>
-      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
         <v>1</v>
       </c>
       <c r="N7" t="n">
         <v>0.15458832444611</v>
       </c>
-      <c r="O7" t="n">
-        <v>0.3168888886666664</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0.4878313187204257</v>
-      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -816,9 +760,7 @@
       <c r="B8" t="n">
         <v>6.35</v>
       </c>
-      <c r="C8" t="n">
-        <v>5.762</v>
-      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
         <v>0.276</v>
       </c>
@@ -840,24 +782,16 @@
       <c r="J8" t="n">
         <v>10.44</v>
       </c>
-      <c r="K8" t="n">
-        <v>4.678</v>
-      </c>
-      <c r="L8" t="n">
-        <v>4.678</v>
-      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="n">
         <v>1</v>
       </c>
       <c r="N8" t="n">
         <v>0.2482040228987069</v>
       </c>
-      <c r="O8" t="n">
-        <v>0.7690595434056761</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0.3227370689655173</v>
-      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -866,9 +800,7 @@
       <c r="B9" t="n">
         <v>7.3</v>
       </c>
-      <c r="C9" t="n">
-        <v>4.036</v>
-      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
         <v>0.381</v>
       </c>
@@ -890,24 +822,16 @@
       <c r="J9" t="n">
         <v>10.44</v>
       </c>
-      <c r="K9" t="n">
-        <v>6.404</v>
-      </c>
-      <c r="L9" t="n">
-        <v>6.404</v>
-      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="n">
         <v>1</v>
       </c>
       <c r="N9" t="n">
         <v>0.08027262416329092</v>
       </c>
-      <c r="O9" t="n">
-        <v>0.204712244495944</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0.3921241954087479</v>
-      </c>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -916,9 +840,7 @@
       <c r="B10" t="n">
         <v>8.300000000000001</v>
       </c>
-      <c r="C10" t="n">
-        <v>3.134</v>
-      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
         <v>0.467</v>
       </c>
@@ -940,24 +862,16 @@
       <c r="J10" t="n">
         <v>10.44</v>
       </c>
-      <c r="K10" t="n">
-        <v>7.305999999999999</v>
-      </c>
-      <c r="L10" t="n">
-        <v>7.305999999999999</v>
-      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="n">
         <v>1</v>
       </c>
       <c r="N10" t="n">
         <v>0.07259358288284798</v>
       </c>
-      <c r="O10" t="n">
-        <v>0.4013303769401335</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0.1808823529290851</v>
-      </c>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -966,9 +880,7 @@
       <c r="B11" t="n">
         <v>9.300000000000001</v>
       </c>
-      <c r="C11" t="n">
-        <v>2.082</v>
-      </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
         <v>0.429</v>
       </c>
@@ -990,24 +902,16 @@
       <c r="J11" t="n">
         <v>10.44</v>
       </c>
-      <c r="K11" t="n">
-        <v>8.358000000000001</v>
-      </c>
-      <c r="L11" t="n">
-        <v>8.358000000000001</v>
-      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
         <v>1</v>
       </c>
       <c r="N11" t="n">
         <v>0.03789106306631612</v>
       </c>
-      <c r="O11" t="n">
-        <v>0.1926489220532315</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0.1966845319583273</v>
-      </c>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1016,9 +920,7 @@
       <c r="B12" t="n">
         <v>21.3</v>
       </c>
-      <c r="C12" t="n">
-        <v>56.204</v>
-      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
         <v>1.489</v>
       </c>
@@ -1037,27 +939,17 @@
       <c r="I12" t="n">
         <v>28.102</v>
       </c>
-      <c r="J12" t="n">
-        <v>145.862</v>
-      </c>
-      <c r="K12" t="n">
-        <v>89.65799999999999</v>
-      </c>
-      <c r="L12" t="n">
-        <v>68.74173270281385</v>
-      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="n">
         <v>1.304273204570096</v>
       </c>
       <c r="N12" t="n">
         <v>0.04532945039001619</v>
       </c>
-      <c r="O12" t="n">
-        <v>0.0500079496883982</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0.9064448887120156</v>
-      </c>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1066,9 +958,7 @@
       <c r="B13" t="n">
         <v>23.3</v>
       </c>
-      <c r="C13" t="n">
-        <v>69.7</v>
-      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
         <v>1.45</v>
       </c>
@@ -1087,27 +977,17 @@
       <c r="I13" t="n">
         <v>34.85</v>
       </c>
-      <c r="J13" t="n">
-        <v>169.662</v>
-      </c>
-      <c r="K13" t="n">
-        <v>99.962</v>
-      </c>
-      <c r="L13" t="n">
-        <v>71.68328608621864</v>
-      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
         <v>1.394495222774365</v>
       </c>
       <c r="N13" t="n">
         <v>0.03949364134873408</v>
       </c>
-      <c r="O13" t="n">
-        <v>0.2301505061303305</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0.1715991939916459</v>
-      </c>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1116,9 +996,7 @@
       <c r="B14" t="n">
         <v>24.3</v>
       </c>
-      <c r="C14" t="n">
-        <v>79.256</v>
-      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
         <v>1.49</v>
       </c>
@@ -1137,27 +1015,17 @@
       <c r="I14" t="n">
         <v>39.628</v>
       </c>
-      <c r="J14" t="n">
-        <v>181.562</v>
-      </c>
-      <c r="K14" t="n">
-        <v>102.306</v>
-      </c>
-      <c r="L14" t="n">
-        <v>70.83332697721671</v>
-      </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
         <v>1.444320129603772</v>
       </c>
       <c r="N14" t="n">
         <v>0.06718569777249125</v>
       </c>
-      <c r="O14" t="n">
-        <v>0.7310155587715322</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0.09190734310141971</v>
-      </c>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1166,9 +1034,7 @@
       <c r="B15" t="n">
         <v>26.3</v>
       </c>
-      <c r="C15" t="n">
-        <v>94.756</v>
-      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
         <v>1.431</v>
       </c>
@@ -1187,27 +1053,17 @@
       <c r="I15" t="n">
         <v>47.378</v>
       </c>
-      <c r="J15" t="n">
-        <v>205.362</v>
-      </c>
-      <c r="K15" t="n">
-        <v>110.606</v>
-      </c>
-      <c r="L15" t="n">
-        <v>71.18688537354446</v>
-      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
         <v>1.553741246292889</v>
       </c>
       <c r="N15" t="n">
         <v>0.01931993821409123</v>
       </c>
-      <c r="O15" t="n">
-        <v>0.9427956950314005</v>
-      </c>
-      <c r="P15" t="n">
-        <v>0.02049217907539105</v>
-      </c>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1216,9 +1072,7 @@
       <c r="B16" t="n">
         <v>27.3</v>
       </c>
-      <c r="C16" t="n">
-        <v>104.982</v>
-      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
         <v>1.394</v>
       </c>
@@ -1237,27 +1091,17 @@
       <c r="I16" t="n">
         <v>52.491</v>
       </c>
-      <c r="J16" t="n">
-        <v>217.262</v>
-      </c>
-      <c r="K16" t="n">
-        <v>112.28</v>
-      </c>
-      <c r="L16" t="n">
-        <v>69.55804999721735</v>
-      </c>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
         <v>1.614191312213205</v>
       </c>
       <c r="N16" t="n">
         <v>0.006430868127268053</v>
       </c>
-      <c r="O16" t="n">
-        <v>0.03274323100733601</v>
-      </c>
-      <c r="P16" t="n">
-        <v>0.1964029794685576</v>
-      </c>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1266,9 +1110,7 @@
       <c r="B17" t="n">
         <v>27.9</v>
       </c>
-      <c r="C17" t="n">
-        <v>113.33</v>
-      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
         <v>1.214</v>
       </c>
@@ -1287,27 +1129,17 @@
       <c r="I17" t="n">
         <v>56.665</v>
       </c>
-      <c r="J17" t="n">
-        <v>224.402</v>
-      </c>
-      <c r="K17" t="n">
-        <v>111.072</v>
-      </c>
-      <c r="L17" t="n">
-        <v>67.20575159889712</v>
-      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
       <c r="M17" t="n">
         <v>1.652715688129031</v>
       </c>
       <c r="N17" t="n">
         <v>0.1912081984223309</v>
       </c>
-      <c r="O17" t="n">
-        <v>0.4018764514209001</v>
-      </c>
-      <c r="P17" t="n">
-        <v>0.4757885109871031</v>
-      </c>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1316,9 +1148,7 @@
       <c r="B18" t="n">
         <v>28.3</v>
       </c>
-      <c r="C18" t="n">
-        <v>119.556</v>
-      </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
         <v>0.9379999999999999</v>
       </c>
@@ -1337,27 +1167,17 @@
       <c r="I18" t="n">
         <v>59.778</v>
       </c>
-      <c r="J18" t="n">
-        <v>236.3</v>
-      </c>
-      <c r="K18" t="n">
-        <v>116.744</v>
-      </c>
-      <c r="L18" t="n">
-        <v>69.04709955852459</v>
-      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
         <v>1.690787893285037</v>
       </c>
       <c r="N18" t="n">
         <v>0.02866889234753486</v>
       </c>
-      <c r="O18" t="n">
-        <v>0.05720446939388425</v>
-      </c>
-      <c r="P18" t="n">
-        <v>0.5011652524933631</v>
-      </c>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1366,9 +1186,7 @@
       <c r="B19" t="n">
         <v>30.5</v>
       </c>
-      <c r="C19" t="n">
-        <v>136.44</v>
-      </c>
+      <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
         <v>0.163</v>
       </c>
@@ -1387,27 +1205,17 @@
       <c r="I19" t="n">
         <v>68.22</v>
       </c>
-      <c r="J19" t="n">
-        <v>314.84</v>
-      </c>
-      <c r="K19" t="n">
-        <v>178.4</v>
-      </c>
-      <c r="L19" t="n">
-        <v>90.54990952549136</v>
-      </c>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
       <c r="M19" t="n">
         <v>1.970184188309733</v>
       </c>
       <c r="N19" t="n">
         <v>0.1700707514016821</v>
       </c>
-      <c r="O19" t="n">
-        <v>0.1579948544036376</v>
-      </c>
-      <c r="P19" t="n">
-        <v>1.076432217008749</v>
-      </c>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1416,9 +1224,7 @@
       <c r="B20" t="n">
         <v>31.5</v>
       </c>
-      <c r="C20" t="n">
-        <v>141.28</v>
-      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
         <v>0.038</v>
       </c>
@@ -1437,27 +1243,17 @@
       <c r="I20" t="n">
         <v>70.64</v>
       </c>
-      <c r="J20" t="n">
-        <v>350.84</v>
-      </c>
-      <c r="K20" t="n">
-        <v>209.56</v>
-      </c>
-      <c r="L20" t="n">
-        <v>99.5918914827856</v>
-      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
         <v>2.104187367866412</v>
       </c>
       <c r="N20" t="n">
         <v>0.02479162268240855</v>
       </c>
-      <c r="O20" t="n">
-        <v>0.03421078934474742</v>
-      </c>
-      <c r="P20" t="n">
-        <v>0.7246726298121779</v>
-      </c>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1480,24 +1276,16 @@
       <c r="J21" t="n">
         <v>360.44</v>
       </c>
-      <c r="K21" t="n">
-        <v>239.965</v>
-      </c>
-      <c r="L21" t="n">
-        <v>98.09957483368598</v>
-      </c>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
         <v>2.446137003211552</v>
       </c>
       <c r="N21" t="n">
         <v>0.0477680122771348</v>
       </c>
-      <c r="O21" t="n">
-        <v>4.297568705589018</v>
-      </c>
-      <c r="P21" t="n">
-        <v>0.01111512474832855</v>
-      </c>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
separated exp calc from model + hplc raw data
</commit_message>
<xml_diff>
--- a/data/Yxs_table.xlsx
+++ b/data/Yxs_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,51 +469,6 @@
           <t>Ethanol [g/L]</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Glucose2 [g/L]</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Glucose [g/L].1</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>added Glucose  [g]</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Consumed_Glucose [g]</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Consumed_Glucose [g/L]</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Volume at each time point</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>mu between direct samples [1/h]</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Yxs [gx/gs]</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>qs 1 - ds/dt/x - [1/h]</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -522,36 +477,21 @@
       <c r="B2" t="n">
         <v>0.2</v>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>10.44</v>
+      </c>
       <c r="D2" t="n">
-        <v>0.167</v>
+        <v>0.34</v>
       </c>
       <c r="E2" t="n">
-        <v>0.037</v>
+        <v>0.08</v>
       </c>
       <c r="F2" t="n">
-        <v>0.007</v>
+        <v>0.02</v>
       </c>
       <c r="G2" t="n">
-        <v>0.079</v>
-      </c>
-      <c r="H2" t="n">
-        <v>5.22</v>
-      </c>
-      <c r="I2" t="n">
-        <v>5.22</v>
-      </c>
-      <c r="J2" t="n">
-        <v>10.44</v>
-      </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
+        <v>0.08</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -560,38 +500,21 @@
       <c r="B3" t="n">
         <v>2.1</v>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>10.36</v>
+      </c>
       <c r="D3" t="n">
-        <v>0.16</v>
+        <v>0.32</v>
       </c>
       <c r="E3" t="n">
-        <v>0.027</v>
+        <v>0.06</v>
       </c>
       <c r="F3" t="n">
-        <v>0.033</v>
+        <v>0.06</v>
       </c>
       <c r="G3" t="n">
-        <v>0.104</v>
-      </c>
-      <c r="H3" t="n">
-        <v>5.176</v>
-      </c>
-      <c r="I3" t="n">
-        <v>5.176</v>
-      </c>
-      <c r="J3" t="n">
-        <v>10.44</v>
-      </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="n">
-        <v>1</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.4676677286516002</v>
-      </c>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
+        <v>0.1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -600,38 +523,21 @@
       <c r="B4" t="n">
         <v>2.3</v>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="n">
+        <v>10.4</v>
+      </c>
       <c r="D4" t="n">
-        <v>0.118</v>
+        <v>0.24</v>
       </c>
       <c r="E4" t="n">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="F4" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.334</v>
-      </c>
-      <c r="H4" t="n">
-        <v>5.198</v>
-      </c>
-      <c r="I4" t="n">
-        <v>5.198</v>
-      </c>
-      <c r="J4" t="n">
-        <v>10.44</v>
-      </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.8825025417389376</v>
-      </c>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
+        <v>0.33</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -640,38 +546,21 @@
       <c r="B5" t="n">
         <v>3.4</v>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>9.380000000000001</v>
+      </c>
       <c r="D5" t="n">
-        <v>0.141</v>
+        <v>0.28</v>
       </c>
       <c r="E5" t="n">
-        <v>0.041</v>
+        <v>0.08</v>
       </c>
       <c r="F5" t="n">
-        <v>0.006</v>
+        <v>0.02</v>
       </c>
       <c r="G5" t="n">
-        <v>0.357</v>
-      </c>
-      <c r="H5" t="n">
-        <v>4.685</v>
-      </c>
-      <c r="I5" t="n">
-        <v>4.685</v>
-      </c>
-      <c r="J5" t="n">
-        <v>10.44</v>
-      </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.5408167273906378</v>
-      </c>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
+        <v>0.36</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -680,38 +569,21 @@
       <c r="B6" t="n">
         <v>4.4</v>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>8.460000000000001</v>
+      </c>
       <c r="D6" t="n">
-        <v>0.187</v>
+        <v>0.38</v>
       </c>
       <c r="E6" t="n">
-        <v>0.044</v>
+        <v>0.08</v>
       </c>
       <c r="F6" t="n">
-        <v>0.024</v>
+        <v>0.04</v>
       </c>
       <c r="G6" t="n">
-        <v>0.148</v>
-      </c>
-      <c r="H6" t="n">
-        <v>4.23</v>
-      </c>
-      <c r="I6" t="n">
-        <v>4.23</v>
-      </c>
-      <c r="J6" t="n">
-        <v>10.44</v>
-      </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="n">
-        <v>1</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.3160748173374999</v>
-      </c>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
+        <v>0.15</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -720,38 +592,21 @@
       <c r="B7" t="n">
         <v>5.35</v>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>6.96</v>
+      </c>
       <c r="D7" t="n">
-        <v>0.21</v>
+        <v>0.42</v>
       </c>
       <c r="E7" t="n">
-        <v>0.041</v>
+        <v>0.08</v>
       </c>
       <c r="F7" t="n">
-        <v>0.058</v>
+        <v>0.12</v>
       </c>
       <c r="G7" t="n">
-        <v>0.146</v>
-      </c>
-      <c r="H7" t="n">
-        <v>3.48</v>
-      </c>
-      <c r="I7" t="n">
-        <v>3.48</v>
-      </c>
-      <c r="J7" t="n">
-        <v>10.44</v>
-      </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="n">
-        <v>1</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.15458832444611</v>
-      </c>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
+        <v>0.15</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -760,38 +615,21 @@
       <c r="B8" t="n">
         <v>6.35</v>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>5.76</v>
+      </c>
       <c r="D8" t="n">
-        <v>0.276</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="E8" t="n">
-        <v>0.043</v>
+        <v>0.08</v>
       </c>
       <c r="F8" t="n">
-        <v>0.122</v>
+        <v>0.24</v>
       </c>
       <c r="G8" t="n">
-        <v>0.128</v>
-      </c>
-      <c r="H8" t="n">
-        <v>2.881</v>
-      </c>
-      <c r="I8" t="n">
-        <v>2.881</v>
-      </c>
-      <c r="J8" t="n">
-        <v>10.44</v>
-      </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="n">
-        <v>1</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.2482040228987069</v>
-      </c>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
+        <v>0.13</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -800,38 +638,21 @@
       <c r="B9" t="n">
         <v>7.3</v>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>4.04</v>
+      </c>
       <c r="D9" t="n">
-        <v>0.381</v>
+        <v>0.76</v>
       </c>
       <c r="E9" t="n">
-        <v>0.005</v>
+        <v>0.02</v>
       </c>
       <c r="F9" t="n">
-        <v>0.23</v>
+        <v>0.46</v>
       </c>
       <c r="G9" t="n">
-        <v>0.141</v>
-      </c>
-      <c r="H9" t="n">
-        <v>2.018</v>
-      </c>
-      <c r="I9" t="n">
-        <v>2.018</v>
-      </c>
-      <c r="J9" t="n">
-        <v>10.44</v>
-      </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="n">
-        <v>1</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0.08027262416329092</v>
-      </c>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
+        <v>0.14</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -840,38 +661,21 @@
       <c r="B10" t="n">
         <v>8.300000000000001</v>
       </c>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>3.14</v>
+      </c>
       <c r="D10" t="n">
-        <v>0.467</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="E10" t="n">
-        <v>0.003</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.339</v>
+        <v>0.68</v>
       </c>
       <c r="G10" t="n">
         <v>0.1</v>
       </c>
-      <c r="H10" t="n">
-        <v>1.567</v>
-      </c>
-      <c r="I10" t="n">
-        <v>1.567</v>
-      </c>
-      <c r="J10" t="n">
-        <v>10.44</v>
-      </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="n">
-        <v>1</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0.07259358288284798</v>
-      </c>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -880,38 +684,21 @@
       <c r="B11" t="n">
         <v>9.300000000000001</v>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>2.08</v>
+      </c>
       <c r="D11" t="n">
-        <v>0.429</v>
+        <v>0.86</v>
       </c>
       <c r="E11" t="n">
-        <v>0.003</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.39</v>
+        <v>0.78</v>
       </c>
       <c r="G11" t="n">
-        <v>0.156</v>
-      </c>
-      <c r="H11" t="n">
-        <v>1.041</v>
-      </c>
-      <c r="I11" t="n">
-        <v>1.041</v>
-      </c>
-      <c r="J11" t="n">
-        <v>10.44</v>
-      </c>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="n">
-        <v>1</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0.03789106306631612</v>
-      </c>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
+        <v>0.16</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -920,36 +707,21 @@
       <c r="B12" t="n">
         <v>21.3</v>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="n">
+        <v>56.2</v>
+      </c>
       <c r="D12" t="n">
-        <v>1.489</v>
+        <v>2.98</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>1.883</v>
+        <v>3.76</v>
       </c>
       <c r="G12" t="n">
-        <v>0.058</v>
-      </c>
-      <c r="H12" t="n">
-        <v>28.102</v>
-      </c>
-      <c r="I12" t="n">
-        <v>28.102</v>
-      </c>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="n">
-        <v>1.304273204570096</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.04532945039001619</v>
-      </c>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
+        <v>0.06</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -958,36 +730,21 @@
       <c r="B13" t="n">
         <v>23.3</v>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="n">
+        <v>69.7</v>
+      </c>
       <c r="D13" t="n">
-        <v>1.45</v>
+        <v>2.9</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>2.078</v>
+        <v>4.16</v>
       </c>
       <c r="G13" t="n">
-        <v>0.048</v>
-      </c>
-      <c r="H13" t="n">
-        <v>34.85</v>
-      </c>
-      <c r="I13" t="n">
-        <v>34.85</v>
-      </c>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="n">
-        <v>1.394495222774365</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0.03949364134873408</v>
-      </c>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
+        <v>0.05</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -996,36 +753,21 @@
       <c r="B14" t="n">
         <v>24.3</v>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="n">
+        <v>79.26000000000001</v>
+      </c>
       <c r="D14" t="n">
-        <v>1.49</v>
+        <v>2.98</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>2.157</v>
+        <v>4.32</v>
       </c>
       <c r="G14" t="n">
-        <v>0.031</v>
-      </c>
-      <c r="H14" t="n">
-        <v>39.628</v>
-      </c>
-      <c r="I14" t="n">
-        <v>39.628</v>
-      </c>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="n">
-        <v>1.444320129603772</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0.06718569777249125</v>
-      </c>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1034,36 +776,21 @@
       <c r="B15" t="n">
         <v>26.3</v>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>94.76000000000001</v>
+      </c>
       <c r="D15" t="n">
-        <v>1.431</v>
+        <v>2.86</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>2.182</v>
+        <v>4.36</v>
       </c>
       <c r="G15" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="H15" t="n">
-        <v>47.378</v>
-      </c>
-      <c r="I15" t="n">
-        <v>47.378</v>
-      </c>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="n">
-        <v>1.553741246292889</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0.01931993821409123</v>
-      </c>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1072,36 +799,21 @@
       <c r="B16" t="n">
         <v>27.3</v>
       </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="n">
+        <v>104.98</v>
+      </c>
       <c r="D16" t="n">
-        <v>1.394</v>
+        <v>2.78</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>2.115</v>
+        <v>4.24</v>
       </c>
       <c r="G16" t="n">
-        <v>0.153</v>
-      </c>
-      <c r="H16" t="n">
-        <v>52.491</v>
-      </c>
-      <c r="I16" t="n">
-        <v>52.491</v>
-      </c>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="n">
-        <v>1.614191312213205</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0.006430868127268053</v>
-      </c>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
+        <v>0.15</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1110,36 +822,21 @@
       <c r="B17" t="n">
         <v>27.9</v>
       </c>
-      <c r="C17" t="inlineStr"/>
+      <c r="C17" t="n">
+        <v>113.34</v>
+      </c>
       <c r="D17" t="n">
-        <v>1.214</v>
+        <v>2.42</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>1.859</v>
+        <v>3.72</v>
       </c>
       <c r="G17" t="n">
-        <v>0.204</v>
-      </c>
-      <c r="H17" t="n">
-        <v>56.665</v>
-      </c>
-      <c r="I17" t="n">
-        <v>56.665</v>
-      </c>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="n">
-        <v>1.652715688129031</v>
-      </c>
-      <c r="N17" t="n">
-        <v>0.1912081984223309</v>
-      </c>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
+        <v>0.2</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1148,36 +845,21 @@
       <c r="B18" t="n">
         <v>28.3</v>
       </c>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="n">
+        <v>119.56</v>
+      </c>
       <c r="D18" t="n">
-        <v>0.9379999999999999</v>
+        <v>1.88</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>1.49</v>
+        <v>2.98</v>
       </c>
       <c r="G18" t="n">
-        <v>0.06900000000000001</v>
-      </c>
-      <c r="H18" t="n">
-        <v>59.778</v>
-      </c>
-      <c r="I18" t="n">
-        <v>59.778</v>
-      </c>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="n">
-        <v>1.690787893285037</v>
-      </c>
-      <c r="N18" t="n">
-        <v>0.02866889234753486</v>
-      </c>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
+        <v>0.07000000000000001</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1186,36 +868,21 @@
       <c r="B19" t="n">
         <v>30.5</v>
       </c>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="n">
+        <v>136.44</v>
+      </c>
       <c r="D19" t="n">
-        <v>0.163</v>
+        <v>0.32</v>
       </c>
       <c r="E19" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F19" t="n">
-        <v>0.355</v>
+        <v>0.72</v>
       </c>
       <c r="G19" t="n">
-        <v>0.041</v>
-      </c>
-      <c r="H19" t="n">
-        <v>150.34</v>
-      </c>
-      <c r="I19" t="n">
-        <v>68.22</v>
-      </c>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="n">
-        <v>1.970184188309733</v>
-      </c>
-      <c r="N19" t="n">
-        <v>0.1700707514016821</v>
-      </c>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
+        <v>0.04</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1224,36 +891,21 @@
       <c r="B20" t="n">
         <v>31.5</v>
       </c>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" t="n">
+        <v>141.28</v>
+      </c>
       <c r="D20" t="n">
-        <v>0.038</v>
+        <v>0.08</v>
       </c>
       <c r="E20" t="n">
-        <v>0.044</v>
+        <v>0.08</v>
       </c>
       <c r="F20" t="n">
-        <v>0.012</v>
+        <v>0.02</v>
       </c>
       <c r="G20" t="n">
-        <v>0.122</v>
-      </c>
-      <c r="H20" t="n">
-        <v>170.96</v>
-      </c>
-      <c r="I20" t="n">
-        <v>70.64</v>
-      </c>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="n">
-        <v>2.104187367866412</v>
-      </c>
-      <c r="N20" t="n">
-        <v>0.02479162268240855</v>
-      </c>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
+        <v>0.12</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1262,30 +914,11 @@
       <c r="B21" t="n">
         <v>42</v>
       </c>
-      <c r="C21" t="n">
-        <v>120.475</v>
-      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="n">
-        <v>120.475</v>
-      </c>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="n">
-        <v>360.44</v>
-      </c>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="n">
-        <v>2.446137003211552</v>
-      </c>
-      <c r="N21" t="n">
-        <v>0.0477680122771348</v>
-      </c>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
change in dCO2dt, parameters & calc of CO2
</commit_message>
<xml_diff>
--- a/data/Yxs_table.xlsx
+++ b/data/Yxs_table.xlsx
@@ -914,7 +914,9 @@
       <c r="B21" t="n">
         <v>42</v>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="n">
+        <v>120.4</v>
+      </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>

</xml_diff>